<commit_message>
terminando a implementacao da analise
</commit_message>
<xml_diff>
--- a/form_responses/responses.xlsx
+++ b/form_responses/responses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -28,13 +28,22 @@
     <t>Não</t>
   </si>
   <si>
+    <t>Hoje é um dia incrível, cheio de boas energias!</t>
+  </si>
+  <si>
     <t>Sim</t>
   </si>
   <si>
-    <t>Muito triste</t>
-  </si>
-  <si>
-    <t>Seilamano</t>
+    <t>Não consigo superar a frustração dessa situação</t>
+  </si>
+  <si>
+    <t>Recebi uma notícia maravilhosa que me deixou radiante!</t>
+  </si>
+  <si>
+    <t>Sinto-me um pouco ansioso com os próximos desafios</t>
+  </si>
+  <si>
+    <t>A tristeza parece persistir, não sei como lidar com isso</t>
   </si>
 </sst>
 </file>
@@ -320,30 +329,72 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>45239.80239603009</v>
+        <v>45242.41506680555</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>45239.80328962963</v>
+        <v>45242.41529898148</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>45242.41548430556</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>45242.41566929399</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>45242.4158944213</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>